<commit_message>
Fixed bug for multi file support- v2.0 ready to use
</commit_message>
<xml_diff>
--- a/src/main/resources/Translations.xlsx
+++ b/src/main/resources/Translations.xlsx
@@ -406,14 +406,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>